<commit_message>
[feat]: showing coordinator name on the excel result
</commit_message>
<xml_diff>
--- a/src/Archivos/cuentaOriginal.xlsx
+++ b/src/Archivos/cuentaOriginal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juancastellon/Documents/proyecto universidad/cuentasDeCobro/src/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851C7AA9-78A8-004F-B5FD-C818858CDCC4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6B5324-A237-4E4D-A7A3-900E5F9A8323}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>iso2008</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>OCTUBRE 2017</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
 </sst>
 </file>
@@ -725,6 +728,191 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -772,193 +960,8 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1360,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="125" zoomScaleNormal="130" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60:P61"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="125" zoomScaleNormal="130" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2717,101 +2720,101 @@
   <sheetData>
     <row r="1" spans="3:33" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="101" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="109" t="s">
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="111"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="83"/>
     </row>
     <row r="3" spans="3:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="97"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="112" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="T3" s="113"/>
-      <c r="U3" s="113"/>
-      <c r="V3" s="113"/>
-      <c r="W3" s="114"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="86"/>
     </row>
     <row r="4" spans="3:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="97"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="115" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="116"/>
-      <c r="U4" s="116"/>
-      <c r="V4" s="116"/>
-      <c r="W4" s="117"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="89"/>
     </row>
     <row r="5" spans="3:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="99"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107"/>
-      <c r="N5" s="107"/>
-      <c r="O5" s="107"/>
-      <c r="P5" s="107"/>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="108"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="80"/>
       <c r="S5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2837,12 +2840,12 @@
         <v>4</v>
       </c>
       <c r="P6" s="35"/>
-      <c r="Q6" s="89"/>
-      <c r="R6" s="89"/>
-      <c r="S6" s="89"/>
-      <c r="T6" s="89"/>
-      <c r="U6" s="89"/>
-      <c r="V6" s="89"/>
+      <c r="Q6" s="90"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
       <c r="W6" s="36"/>
     </row>
     <row r="7" spans="3:33" ht="16" x14ac:dyDescent="0.2">
@@ -2872,52 +2875,52 @@
     </row>
     <row r="8" spans="3:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="33"/>
-      <c r="D8" s="90" t="s">
+      <c r="D8" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
-      <c r="O8" s="90"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="90"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="90"/>
-      <c r="U8" s="90"/>
-      <c r="V8" s="90"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="91"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="91"/>
+      <c r="S8" s="91"/>
+      <c r="T8" s="91"/>
+      <c r="U8" s="91"/>
+      <c r="V8" s="91"/>
       <c r="W8" s="36"/>
     </row>
     <row r="9" spans="3:33" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="33"/>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="76"/>
+      <c r="S9" s="76"/>
+      <c r="T9" s="76"/>
+      <c r="U9" s="76"/>
+      <c r="V9" s="76"/>
       <c r="W9" s="36"/>
     </row>
     <row r="10" spans="3:33" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2945,27 +2948,27 @@
     </row>
     <row r="11" spans="3:33" ht="16" x14ac:dyDescent="0.2">
       <c r="C11" s="33"/>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="70"/>
-      <c r="M11" s="70"/>
-      <c r="N11" s="70"/>
-      <c r="O11" s="70"/>
-      <c r="P11" s="70"/>
-      <c r="Q11" s="70"/>
-      <c r="R11" s="70"/>
-      <c r="S11" s="70"/>
-      <c r="T11" s="70"/>
-      <c r="U11" s="70"/>
-      <c r="V11" s="70"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="76"/>
+      <c r="R11" s="76"/>
+      <c r="S11" s="76"/>
+      <c r="T11" s="76"/>
+      <c r="U11" s="76"/>
+      <c r="V11" s="76"/>
       <c r="W11" s="36"/>
     </row>
     <row r="12" spans="3:33" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2993,27 +2996,27 @@
     </row>
     <row r="13" spans="3:33" ht="16" x14ac:dyDescent="0.2">
       <c r="C13" s="33"/>
-      <c r="D13" s="94" t="s">
+      <c r="D13" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="94"/>
-      <c r="F13" s="94"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="92"/>
-      <c r="O13" s="92"/>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="92"/>
-      <c r="S13" s="92"/>
-      <c r="T13" s="92"/>
-      <c r="U13" s="92"/>
-      <c r="V13" s="93"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="93"/>
+      <c r="M13" s="93"/>
+      <c r="N13" s="93"/>
+      <c r="O13" s="93"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="93"/>
+      <c r="R13" s="93"/>
+      <c r="S13" s="93"/>
+      <c r="T13" s="93"/>
+      <c r="U13" s="93"/>
+      <c r="V13" s="94"/>
       <c r="W13" s="36"/>
     </row>
     <row r="14" spans="3:33" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3041,17 +3044,17 @@
     </row>
     <row r="15" spans="3:33" ht="16" x14ac:dyDescent="0.2">
       <c r="C15" s="33"/>
-      <c r="D15" s="125" t="s">
+      <c r="D15" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="121"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="59"/>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="17"/>
@@ -3101,27 +3104,27 @@
     </row>
     <row r="17" spans="3:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="33"/>
-      <c r="D17" s="94" t="s">
+      <c r="D17" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="124"/>
-      <c r="J17" s="124"/>
-      <c r="K17" s="124"/>
-      <c r="L17" s="124"/>
-      <c r="M17" s="124"/>
-      <c r="N17" s="124"/>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="124"/>
-      <c r="R17" s="124"/>
-      <c r="S17" s="124"/>
-      <c r="T17" s="124"/>
-      <c r="U17" s="124"/>
-      <c r="V17" s="124"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="62"/>
       <c r="W17" s="36"/>
     </row>
     <row r="18" spans="3:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3149,27 +3152,27 @@
     </row>
     <row r="19" spans="3:23" ht="16" x14ac:dyDescent="0.2">
       <c r="C19" s="33"/>
-      <c r="D19" s="94" t="s">
+      <c r="D19" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="122"/>
-      <c r="K19" s="122"/>
-      <c r="L19" s="122"/>
-      <c r="M19" s="122"/>
-      <c r="N19" s="122"/>
-      <c r="O19" s="122"/>
-      <c r="P19" s="122"/>
-      <c r="Q19" s="122"/>
-      <c r="R19" s="122"/>
-      <c r="S19" s="122"/>
-      <c r="T19" s="122"/>
-      <c r="U19" s="122"/>
-      <c r="V19" s="122"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="60"/>
+      <c r="S19" s="60"/>
+      <c r="T19" s="60"/>
+      <c r="U19" s="60"/>
+      <c r="V19" s="60"/>
       <c r="W19" s="36"/>
     </row>
     <row r="20" spans="3:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3199,27 +3202,27 @@
     </row>
     <row r="21" spans="3:23" ht="16" x14ac:dyDescent="0.2">
       <c r="C21" s="40"/>
-      <c r="D21" s="126" t="s">
+      <c r="D21" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-      <c r="N21" s="118"/>
-      <c r="O21" s="118"/>
-      <c r="P21" s="118"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="118"/>
-      <c r="S21" s="118"/>
-      <c r="T21" s="118"/>
-      <c r="U21" s="118"/>
-      <c r="V21" s="118"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+      <c r="V21" s="56"/>
       <c r="W21" s="36"/>
     </row>
     <row r="22" spans="3:23" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -3247,8 +3250,8 @@
     </row>
     <row r="23" spans="3:23" ht="25" x14ac:dyDescent="0.2">
       <c r="C23" s="33"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="113"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -3270,25 +3273,25 @@
     </row>
     <row r="24" spans="3:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="33"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="70"/>
-      <c r="O24" s="70"/>
-      <c r="P24" s="70"/>
-      <c r="Q24" s="70"/>
-      <c r="R24" s="70"/>
-      <c r="S24" s="70"/>
-      <c r="T24" s="70"/>
-      <c r="U24" s="70"/>
-      <c r="V24" s="70"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
+      <c r="N24" s="76"/>
+      <c r="O24" s="76"/>
+      <c r="P24" s="76"/>
+      <c r="Q24" s="76"/>
+      <c r="R24" s="76"/>
+      <c r="S24" s="76"/>
+      <c r="T24" s="76"/>
+      <c r="U24" s="76"/>
+      <c r="V24" s="76"/>
       <c r="W24" s="36"/>
     </row>
     <row r="25" spans="3:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3316,71 +3319,71 @@
     </row>
     <row r="26" spans="3:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="33"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
-      <c r="M26" s="79"/>
-      <c r="N26" s="79"/>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="79"/>
-      <c r="T26" s="79"/>
-      <c r="U26" s="79"/>
-      <c r="V26" s="79"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="97"/>
+      <c r="K26" s="97"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
+      <c r="P26" s="97"/>
+      <c r="Q26" s="97"/>
+      <c r="R26" s="97"/>
+      <c r="S26" s="97"/>
+      <c r="T26" s="97"/>
+      <c r="U26" s="97"/>
+      <c r="V26" s="97"/>
       <c r="W26" s="36"/>
     </row>
     <row r="27" spans="3:23" ht="16" x14ac:dyDescent="0.2">
       <c r="C27" s="33"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="79"/>
-      <c r="O27" s="79"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="79"/>
-      <c r="S27" s="79"/>
-      <c r="T27" s="79"/>
-      <c r="U27" s="79"/>
-      <c r="V27" s="79"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="97"/>
+      <c r="O27" s="97"/>
+      <c r="P27" s="97"/>
+      <c r="Q27" s="97"/>
+      <c r="R27" s="97"/>
+      <c r="S27" s="97"/>
+      <c r="T27" s="97"/>
+      <c r="U27" s="97"/>
+      <c r="V27" s="97"/>
       <c r="W27" s="36"/>
     </row>
     <row r="28" spans="3:23" ht="16" x14ac:dyDescent="0.2">
       <c r="C28" s="33"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="79"/>
-      <c r="O28" s="79"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="79"/>
-      <c r="S28" s="79"/>
-      <c r="T28" s="79"/>
-      <c r="U28" s="79"/>
-      <c r="V28" s="79"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="97"/>
+      <c r="N28" s="97"/>
+      <c r="O28" s="97"/>
+      <c r="P28" s="97"/>
+      <c r="Q28" s="97"/>
+      <c r="R28" s="97"/>
+      <c r="S28" s="97"/>
+      <c r="T28" s="97"/>
+      <c r="U28" s="97"/>
+      <c r="V28" s="97"/>
       <c r="W28" s="36"/>
     </row>
     <row r="29" spans="3:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3435,23 +3438,23 @@
         <v>9</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="82"/>
-      <c r="I31" s="82"/>
-      <c r="J31" s="82"/>
-      <c r="K31" s="82"/>
-      <c r="L31" s="82"/>
-      <c r="M31" s="82"/>
-      <c r="N31" s="82"/>
-      <c r="O31" s="82"/>
-      <c r="P31" s="82"/>
-      <c r="Q31" s="82"/>
-      <c r="R31" s="82"/>
-      <c r="S31" s="82"/>
-      <c r="T31" s="82"/>
-      <c r="U31" s="82"/>
-      <c r="V31" s="82"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="102"/>
+      <c r="I31" s="102"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="102"/>
+      <c r="L31" s="102"/>
+      <c r="M31" s="102"/>
+      <c r="N31" s="102"/>
+      <c r="O31" s="102"/>
+      <c r="P31" s="102"/>
+      <c r="Q31" s="102"/>
+      <c r="R31" s="102"/>
+      <c r="S31" s="102"/>
+      <c r="T31" s="102"/>
+      <c r="U31" s="102"/>
+      <c r="V31" s="102"/>
       <c r="W31" s="36"/>
     </row>
     <row r="32" spans="3:23" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3481,10 +3484,10 @@
       <c r="C33" s="33"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="74" t="s">
+      <c r="F33" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="76"/>
+      <c r="G33" s="101"/>
       <c r="H33" s="54" t="s">
         <v>11</v>
       </c>
@@ -3492,17 +3495,17 @@
       <c r="J33" s="53"/>
       <c r="K33" s="53"/>
       <c r="L33" s="53"/>
-      <c r="M33" s="80" t="s">
+      <c r="M33" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="81" t="s">
+      <c r="N33" s="99"/>
+      <c r="O33" s="99"/>
+      <c r="P33" s="99"/>
+      <c r="Q33" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="R33" s="81"/>
-      <c r="S33" s="81"/>
+      <c r="R33" s="99"/>
+      <c r="S33" s="99"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
@@ -3522,20 +3525,20 @@
       <c r="C34" s="33"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="72"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="105"/>
       <c r="H34" s="26"/>
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
       <c r="K34" s="20"/>
       <c r="L34" s="30"/>
-      <c r="M34" s="71"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="72"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84"/>
-      <c r="S34" s="85"/>
+      <c r="M34" s="103"/>
+      <c r="N34" s="104"/>
+      <c r="O34" s="104"/>
+      <c r="P34" s="105"/>
+      <c r="Q34" s="106"/>
+      <c r="R34" s="107"/>
+      <c r="S34" s="108"/>
       <c r="T34" s="21"/>
       <c r="U34" s="5"/>
       <c r="V34" s="5"/>
@@ -3555,20 +3558,20 @@
       <c r="C35" s="33"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="72"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="105"/>
       <c r="H35" s="28"/>
       <c r="I35" s="20"/>
       <c r="J35" s="51"/>
       <c r="K35" s="20"/>
       <c r="L35" s="30"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="73"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="72"/>
-      <c r="Q35" s="86"/>
-      <c r="R35" s="87"/>
-      <c r="S35" s="88"/>
+      <c r="M35" s="103"/>
+      <c r="N35" s="104"/>
+      <c r="O35" s="104"/>
+      <c r="P35" s="105"/>
+      <c r="Q35" s="109"/>
+      <c r="R35" s="110"/>
+      <c r="S35" s="111"/>
       <c r="T35" s="22"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
@@ -3588,20 +3591,20 @@
       <c r="C36" s="33"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="72"/>
+      <c r="F36" s="103"/>
+      <c r="G36" s="105"/>
       <c r="H36" s="26"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
       <c r="L36" s="30"/>
-      <c r="M36" s="71"/>
-      <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="72"/>
-      <c r="Q36" s="74"/>
-      <c r="R36" s="75"/>
-      <c r="S36" s="76"/>
+      <c r="M36" s="103"/>
+      <c r="N36" s="104"/>
+      <c r="O36" s="104"/>
+      <c r="P36" s="105"/>
+      <c r="Q36" s="100"/>
+      <c r="R36" s="126"/>
+      <c r="S36" s="101"/>
       <c r="T36" s="22"/>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
@@ -3621,20 +3624,20 @@
       <c r="C37" s="33"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="72"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="105"/>
       <c r="H37" s="28"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
       <c r="K37" s="20"/>
       <c r="L37" s="30"/>
-      <c r="M37" s="71"/>
-      <c r="N37" s="73"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="75"/>
-      <c r="S37" s="76"/>
+      <c r="M37" s="103"/>
+      <c r="N37" s="104"/>
+      <c r="O37" s="104"/>
+      <c r="P37" s="105"/>
+      <c r="Q37" s="100"/>
+      <c r="R37" s="126"/>
+      <c r="S37" s="101"/>
       <c r="T37" s="23"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
@@ -3692,10 +3695,10 @@
       <c r="F39" s="52"/>
       <c r="G39" s="5"/>
       <c r="H39" s="24"/>
-      <c r="I39" s="78" t="s">
+      <c r="I39" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="78"/>
+      <c r="J39" s="96"/>
       <c r="K39" s="29"/>
       <c r="L39" s="55" t="s">
         <v>14</v>
@@ -3704,9 +3707,9 @@
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
-      <c r="Q39" s="77"/>
-      <c r="R39" s="77"/>
-      <c r="S39" s="77"/>
+      <c r="Q39" s="95"/>
+      <c r="R39" s="95"/>
+      <c r="S39" s="95"/>
       <c r="T39" s="30"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
@@ -3767,12 +3770,12 @@
       <c r="I41" s="29"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="65"/>
-      <c r="M41" s="66"/>
-      <c r="N41" s="66"/>
-      <c r="O41" s="66"/>
-      <c r="P41" s="66"/>
-      <c r="Q41" s="67"/>
+      <c r="L41" s="121"/>
+      <c r="M41" s="122"/>
+      <c r="N41" s="122"/>
+      <c r="O41" s="122"/>
+      <c r="P41" s="122"/>
+      <c r="Q41" s="123"/>
       <c r="R41" s="30"/>
       <c r="S41" s="30"/>
       <c r="T41" s="30"/>
@@ -3802,12 +3805,12 @@
       <c r="I42" s="29"/>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="65"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="66"/>
-      <c r="O42" s="66"/>
-      <c r="P42" s="66"/>
-      <c r="Q42" s="67"/>
+      <c r="L42" s="121"/>
+      <c r="M42" s="122"/>
+      <c r="N42" s="122"/>
+      <c r="O42" s="122"/>
+      <c r="P42" s="122"/>
+      <c r="Q42" s="123"/>
       <c r="R42" s="30"/>
       <c r="S42" s="30"/>
       <c r="T42" s="30"/>
@@ -3837,12 +3840,12 @@
       <c r="I43" s="29"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="65"/>
-      <c r="M43" s="66"/>
-      <c r="N43" s="66"/>
-      <c r="O43" s="66"/>
-      <c r="P43" s="66"/>
-      <c r="Q43" s="67"/>
+      <c r="L43" s="121"/>
+      <c r="M43" s="122"/>
+      <c r="N43" s="122"/>
+      <c r="O43" s="122"/>
+      <c r="P43" s="122"/>
+      <c r="Q43" s="123"/>
       <c r="R43" s="30"/>
       <c r="S43" s="30"/>
       <c r="T43" s="30"/>
@@ -3941,27 +3944,27 @@
     </row>
     <row r="47" spans="3:33" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="33"/>
-      <c r="D47" s="70" t="s">
+      <c r="D47" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="70"/>
-      <c r="N47" s="70"/>
-      <c r="O47" s="70"/>
-      <c r="P47" s="70"/>
-      <c r="Q47" s="70"/>
-      <c r="R47" s="70"/>
-      <c r="S47" s="70"/>
-      <c r="T47" s="70"/>
-      <c r="U47" s="70"/>
-      <c r="V47" s="70"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="76"/>
+      <c r="O47" s="76"/>
+      <c r="P47" s="76"/>
+      <c r="Q47" s="76"/>
+      <c r="R47" s="76"/>
+      <c r="S47" s="76"/>
+      <c r="T47" s="76"/>
+      <c r="U47" s="76"/>
+      <c r="V47" s="76"/>
       <c r="W47" s="36"/>
     </row>
     <row r="48" spans="3:33" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4063,20 +4066,20 @@
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="69"/>
-      <c r="I52" s="69"/>
-      <c r="J52" s="69"/>
-      <c r="K52" s="69"/>
-      <c r="L52" s="69"/>
-      <c r="M52" s="69"/>
-      <c r="N52" s="69"/>
-      <c r="O52" s="69"/>
-      <c r="P52" s="69"/>
-      <c r="Q52" s="69"/>
-      <c r="R52" s="69"/>
-      <c r="S52" s="69"/>
-      <c r="T52" s="69"/>
+      <c r="G52" s="124"/>
+      <c r="H52" s="125"/>
+      <c r="I52" s="125"/>
+      <c r="J52" s="125"/>
+      <c r="K52" s="125"/>
+      <c r="L52" s="125"/>
+      <c r="M52" s="125"/>
+      <c r="N52" s="125"/>
+      <c r="O52" s="125"/>
+      <c r="P52" s="125"/>
+      <c r="Q52" s="125"/>
+      <c r="R52" s="125"/>
+      <c r="S52" s="125"/>
+      <c r="T52" s="125"/>
       <c r="U52" s="5" t="s">
         <v>20</v>
       </c>
@@ -4132,27 +4135,27 @@
       <c r="W54" s="38"/>
     </row>
     <row r="55" spans="3:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="58"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="59"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="59"/>
-      <c r="K55" s="59"/>
-      <c r="L55" s="59"/>
-      <c r="M55" s="59"/>
-      <c r="N55" s="59"/>
-      <c r="O55" s="59"/>
-      <c r="P55" s="59"/>
-      <c r="Q55" s="59"/>
-      <c r="R55" s="59"/>
-      <c r="S55" s="59"/>
-      <c r="T55" s="59"/>
-      <c r="U55" s="59"/>
-      <c r="V55" s="59"/>
-      <c r="W55" s="60"/>
+      <c r="C55" s="114"/>
+      <c r="D55" s="115"/>
+      <c r="E55" s="115"/>
+      <c r="F55" s="115"/>
+      <c r="G55" s="115"/>
+      <c r="H55" s="115"/>
+      <c r="I55" s="115"/>
+      <c r="J55" s="115"/>
+      <c r="K55" s="115"/>
+      <c r="L55" s="115"/>
+      <c r="M55" s="115"/>
+      <c r="N55" s="115"/>
+      <c r="O55" s="115"/>
+      <c r="P55" s="115"/>
+      <c r="Q55" s="115"/>
+      <c r="R55" s="115"/>
+      <c r="S55" s="115"/>
+      <c r="T55" s="115"/>
+      <c r="U55" s="115"/>
+      <c r="V55" s="115"/>
+      <c r="W55" s="116"/>
     </row>
     <row r="56" spans="3:23" ht="16" x14ac:dyDescent="0.2">
       <c r="C56" s="33"/>
@@ -4248,31 +4251,31 @@
     </row>
     <row r="60" spans="3:23" ht="16" x14ac:dyDescent="0.2">
       <c r="C60" s="33"/>
-      <c r="D60" s="61" t="s">
+      <c r="D60" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="E60" s="61"/>
-      <c r="F60" s="61"/>
-      <c r="G60" s="61"/>
-      <c r="H60" s="61"/>
+      <c r="E60" s="117"/>
+      <c r="F60" s="117"/>
+      <c r="G60" s="117"/>
+      <c r="H60" s="117"/>
       <c r="I60" s="5"/>
-      <c r="J60" s="62" t="s">
+      <c r="J60" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="K60" s="62"/>
-      <c r="L60" s="62"/>
-      <c r="M60" s="62"/>
-      <c r="N60" s="62"/>
-      <c r="O60" s="62"/>
-      <c r="P60" s="62"/>
-      <c r="Q60" s="64" t="s">
+      <c r="K60" s="118"/>
+      <c r="L60" s="118"/>
+      <c r="M60" s="118"/>
+      <c r="N60" s="118"/>
+      <c r="O60" s="118"/>
+      <c r="P60" s="118"/>
+      <c r="Q60" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="R60" s="64"/>
-      <c r="S60" s="64"/>
-      <c r="T60" s="64"/>
-      <c r="U60" s="64"/>
-      <c r="V60" s="64"/>
+      <c r="R60" s="120"/>
+      <c r="S60" s="120"/>
+      <c r="T60" s="120"/>
+      <c r="U60" s="120"/>
+      <c r="V60" s="120"/>
       <c r="W60" s="36"/>
     </row>
     <row r="61" spans="3:23" x14ac:dyDescent="0.2">
@@ -4283,13 +4286,13 @@
       <c r="G61" s="16"/>
       <c r="H61" s="16"/>
       <c r="I61" s="16"/>
-      <c r="J61" s="63"/>
-      <c r="K61" s="63"/>
-      <c r="L61" s="63"/>
-      <c r="M61" s="63"/>
-      <c r="N61" s="63"/>
-      <c r="O61" s="63"/>
-      <c r="P61" s="63"/>
+      <c r="J61" s="119"/>
+      <c r="K61" s="119"/>
+      <c r="L61" s="119"/>
+      <c r="M61" s="119"/>
+      <c r="N61" s="119"/>
+      <c r="O61" s="119"/>
+      <c r="P61" s="119"/>
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
       <c r="S61" s="16"/>
@@ -4300,6 +4303,9 @@
     </row>
     <row r="62" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C62" s="43"/>
+      <c r="J62" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="W62" s="44"/>
     </row>
     <row r="63" spans="3:23" x14ac:dyDescent="0.2">
@@ -4343,39 +4349,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="H21:V21"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H19:V19"/>
-    <mergeCell ref="H17:V17"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="C2:G5"/>
-    <mergeCell ref="H2:R5"/>
-    <mergeCell ref="S2:W2"/>
-    <mergeCell ref="S3:W3"/>
-    <mergeCell ref="S4:W4"/>
-    <mergeCell ref="Q6:V6"/>
-    <mergeCell ref="D8:V8"/>
-    <mergeCell ref="D9:V9"/>
-    <mergeCell ref="D11:V11"/>
-    <mergeCell ref="H13:V13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="D24:V24"/>
-    <mergeCell ref="D26:V28"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F31:V31"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="Q35:S35"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="C55:W55"/>
     <mergeCell ref="D60:H60"/>
@@ -4392,6 +4365,39 @@
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="Q36:S36"/>
     <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="D24:V24"/>
+    <mergeCell ref="D26:V28"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F31:V31"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="Q6:V6"/>
+    <mergeCell ref="D8:V8"/>
+    <mergeCell ref="D9:V9"/>
+    <mergeCell ref="D11:V11"/>
+    <mergeCell ref="H13:V13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="C2:G5"/>
+    <mergeCell ref="H2:R5"/>
+    <mergeCell ref="S2:W2"/>
+    <mergeCell ref="S3:W3"/>
+    <mergeCell ref="S4:W4"/>
+    <mergeCell ref="H21:V21"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H19:V19"/>
+    <mergeCell ref="H17:V17"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>